<commit_message>
[SingleJobInvoice] : Screenshot Script Added
</commit_message>
<xml_diff>
--- a/Invoice _TestData/IFF_INVOICE_TEST_DATA.xlsx
+++ b/Invoice _TestData/IFF_INVOICE_TEST_DATA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="basicDetails" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="336">
   <si>
     <t>Basic Details</t>
   </si>
@@ -961,49 +961,79 @@
     <t>Invoice against service Air Freight Import</t>
   </si>
   <si>
-    <t>25-Jun-2023</t>
-  </si>
-  <si>
     <t>30-Jun-2023</t>
   </si>
   <si>
     <t>Invoice Ref</t>
   </si>
   <si>
-    <t>29-Jun-2023</t>
-  </si>
-  <si>
     <t>Original Bill of Lading</t>
   </si>
   <si>
     <t>Telex Release</t>
   </si>
   <si>
-    <t>20-Jun-2023</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>cde</t>
-  </si>
-  <si>
-    <t>MUM/BKG/AEC/00012/2122-48</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFI/00172/23-24</t>
-  </si>
-  <si>
     <t>Overseas Tax</t>
   </si>
   <si>
     <t>Bill of Supply</t>
   </si>
   <si>
-    <t>CHN/BKG/AFE/00173/23-24</t>
+    <t>RAMCO INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>BANK OF INDIA(11111112222)/23123/INR</t>
+  </si>
+  <si>
+    <t>STATE BANK OF INDIA(255000552232112)/22156132122/INR</t>
+  </si>
+  <si>
+    <t>ZOYA CONTAINER LINE</t>
+  </si>
+  <si>
+    <t>23-Jun-2023</t>
+  </si>
+  <si>
+    <t>06-Jul-2023</t>
+  </si>
+  <si>
+    <t>04-Jul-2023</t>
+  </si>
+  <si>
+    <t>28-Jun-2023</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>fff</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFI/00191/23-24</t>
+  </si>
+  <si>
+    <t>01-Jul-2023</t>
+  </si>
+  <si>
+    <t>10-Jul-2023</t>
+  </si>
+  <si>
+    <t>MUM/BKG/AEC/00012/2122-60</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFE/00192/23-24</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1559,70 +1589,23 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1631,7 +1614,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1865,11 +1848,72 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1883,38 +1927,14 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2219,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2327,11 +2347,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="111" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="113"/>
     </row>
     <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
@@ -2373,10 +2393,10 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="87"/>
+      <c r="C6" s="110"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -2452,20 +2472,20 @@
         <v>21</v>
       </c>
       <c r="X7" s="83" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y7" s="77"/>
       <c r="Z7" s="77"/>
     </row>
-    <row r="8" spans="1:26" s="45" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" s="45" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="44">
         <v>7</v>
       </c>
       <c r="B8" s="63">
         <v>1</v>
       </c>
-      <c r="C8" s="85" t="s">
-        <v>325</v>
+      <c r="C8" s="91" t="s">
+        <v>335</v>
       </c>
       <c r="D8" s="64" t="s">
         <v>24</v>
@@ -2510,19 +2530,19 @@
         <v>308</v>
       </c>
       <c r="R8" s="67" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="S8" s="67" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="T8" s="68" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U8" s="65" t="s">
         <v>25</v>
       </c>
       <c r="V8" s="68" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="W8" s="80" t="s">
         <v>24</v>
@@ -2531,15 +2551,15 @@
       <c r="Y8" s="78"/>
       <c r="Z8" s="78"/>
     </row>
-    <row r="9" spans="1:26" s="45" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="43">
         <v>8</v>
       </c>
       <c r="B9" s="46">
         <v>2</v>
       </c>
-      <c r="C9" s="86" t="s">
-        <v>321</v>
+      <c r="C9" s="92" t="s">
+        <v>334</v>
       </c>
       <c r="D9" s="48" t="s">
         <v>24</v>
@@ -2584,19 +2604,19 @@
         <v>309</v>
       </c>
       <c r="R9" s="52" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="S9" s="52" t="s">
-        <v>311</v>
-      </c>
-      <c r="T9" s="68" t="s">
-        <v>316</v>
+        <v>323</v>
+      </c>
+      <c r="T9" s="87" t="s">
+        <v>314</v>
       </c>
       <c r="U9" s="50" t="s">
         <v>25</v>
       </c>
       <c r="V9" s="51" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="W9" s="81" t="s">
         <v>24</v>
@@ -2609,13 +2629,13 @@
       <c r="A10" s="43">
         <v>9</v>
       </c>
-      <c r="B10" s="59">
+      <c r="B10" s="89">
         <v>3</v>
       </c>
-      <c r="C10" s="91" t="s">
-        <v>322</v>
-      </c>
-      <c r="D10" s="60" t="s">
+      <c r="C10" s="93" t="s">
+        <v>331</v>
+      </c>
+      <c r="D10" s="90" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="60" t="s">
@@ -2658,19 +2678,19 @@
         <v>310</v>
       </c>
       <c r="R10" s="62" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="S10" s="62" t="s">
-        <v>312</v>
-      </c>
-      <c r="T10" s="68" t="s">
-        <v>316</v>
+        <v>333</v>
+      </c>
+      <c r="T10" s="88" t="s">
+        <v>314</v>
       </c>
       <c r="U10" s="59" t="s">
         <v>25</v>
       </c>
       <c r="V10" s="61" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="W10" s="82" t="s">
         <v>24</v>
@@ -2678,6 +2698,207 @@
       <c r="X10" s="84"/>
       <c r="Y10" s="78"/>
       <c r="Z10" s="78"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B11" s="103">
+        <v>4</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="104" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="94" t="s">
+        <v>291</v>
+      </c>
+      <c r="H11" s="106" t="s">
+        <v>306</v>
+      </c>
+      <c r="I11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="106" t="s">
+        <v>306</v>
+      </c>
+      <c r="K11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="106" t="s">
+        <v>307</v>
+      </c>
+      <c r="M11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="106" t="s">
+        <v>310</v>
+      </c>
+      <c r="R11" s="107" t="s">
+        <v>324</v>
+      </c>
+      <c r="S11" s="107" t="s">
+        <v>311</v>
+      </c>
+      <c r="T11" s="108" t="s">
+        <v>314</v>
+      </c>
+      <c r="U11" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="V11" s="106" t="s">
+        <v>328</v>
+      </c>
+      <c r="W11" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" s="84"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B12" s="94">
+        <v>5</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="94" t="s">
+        <v>291</v>
+      </c>
+      <c r="H12" s="106" t="s">
+        <v>317</v>
+      </c>
+      <c r="I12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="106" t="s">
+        <v>317</v>
+      </c>
+      <c r="K12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="106" t="s">
+        <v>307</v>
+      </c>
+      <c r="M12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="106" t="s">
+        <v>310</v>
+      </c>
+      <c r="R12" s="107" t="s">
+        <v>321</v>
+      </c>
+      <c r="S12" s="107" t="s">
+        <v>311</v>
+      </c>
+      <c r="T12" s="108" t="s">
+        <v>314</v>
+      </c>
+      <c r="U12" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="V12" s="106" t="s">
+        <v>329</v>
+      </c>
+      <c r="W12" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="X12" s="84"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B13" s="94">
+        <v>6</v>
+      </c>
+      <c r="C13" s="86"/>
+      <c r="D13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="94" t="s">
+        <v>291</v>
+      </c>
+      <c r="H13" s="106" t="s">
+        <v>320</v>
+      </c>
+      <c r="I13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="106" t="s">
+        <v>320</v>
+      </c>
+      <c r="K13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="106" t="s">
+        <v>307</v>
+      </c>
+      <c r="M13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="106" t="s">
+        <v>310</v>
+      </c>
+      <c r="R13" s="107" t="s">
+        <v>321</v>
+      </c>
+      <c r="S13" s="107" t="s">
+        <v>311</v>
+      </c>
+      <c r="T13" s="108" t="s">
+        <v>314</v>
+      </c>
+      <c r="U13" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="V13" s="106" t="s">
+        <v>330</v>
+      </c>
+      <c r="W13" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="X13" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2685,13 +2906,13 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G13">
       <formula1>"Customer,Vendor,Service Partner"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U13">
       <formula1>"GST"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T8:T10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T8:T13">
       <formula1>"Select,Original Bill of Lading,Telex Release,Bank Guarantee,Personal Guarantee"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2705,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GC10"/>
+  <dimension ref="A1:GC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3600,7 +3821,7 @@
       <c r="J7" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="92" t="s">
+      <c r="K7" s="85" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="41"/>
@@ -3614,10 +3835,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D8" s="70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="71" t="s">
         <v>34</v>
@@ -3629,10 +3850,10 @@
         <v>51</v>
       </c>
       <c r="H8" s="72">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="72">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="J8" s="65" t="s">
         <v>227</v>
@@ -3651,10 +3872,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D9" s="50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="47" t="s">
         <v>232</v>
@@ -3666,7 +3887,7 @@
         <v>55</v>
       </c>
       <c r="H9" s="55">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I9" s="55">
         <v>20</v>
@@ -3680,42 +3901,138 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:185" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:185" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="93">
+      <c r="B10" s="95">
         <v>3</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="96" t="s">
         <v>231</v>
       </c>
       <c r="D10" s="95">
-        <v>3</v>
-      </c>
-      <c r="E10" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="97" t="s">
         <v>233</v>
       </c>
-      <c r="F10" s="96" t="s">
+      <c r="F10" s="97" t="s">
         <v>301</v>
       </c>
-      <c r="G10" s="97" t="s">
+      <c r="G10" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="98">
-        <v>7</v>
-      </c>
-      <c r="I10" s="98">
+      <c r="H10" s="99">
+        <v>12</v>
+      </c>
+      <c r="I10" s="99">
         <v>30</v>
       </c>
-      <c r="J10" s="94" t="s">
+      <c r="J10" s="96" t="s">
         <v>229</v>
       </c>
-      <c r="K10" s="99" t="s">
+      <c r="K10" s="100" t="s">
         <v>304</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:185" x14ac:dyDescent="0.3">
+      <c r="B11" s="94">
+        <v>4</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>316</v>
+      </c>
+      <c r="D11" s="94">
+        <v>6</v>
+      </c>
+      <c r="E11" s="101" t="s">
+        <v>233</v>
+      </c>
+      <c r="F11" s="101" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="102">
+        <v>14</v>
+      </c>
+      <c r="I11" s="102">
+        <v>30</v>
+      </c>
+      <c r="J11" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="K11" s="101" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:185" x14ac:dyDescent="0.3">
+      <c r="B12" s="94">
+        <v>5</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>315</v>
+      </c>
+      <c r="D12" s="94">
+        <v>5</v>
+      </c>
+      <c r="E12" s="101" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="101" t="s">
+        <v>301</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="102">
+        <v>16</v>
+      </c>
+      <c r="I12" s="102">
+        <v>30</v>
+      </c>
+      <c r="J12" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" s="101" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:185" x14ac:dyDescent="0.3">
+      <c r="B13" s="94">
+        <v>6</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="94">
+        <v>6</v>
+      </c>
+      <c r="E13" s="101" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="101" t="s">
+        <v>301</v>
+      </c>
+      <c r="G13" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="102">
+        <v>18</v>
+      </c>
+      <c r="I13" s="102">
+        <v>30</v>
+      </c>
+      <c r="J13" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="K13" s="101" t="s">
+        <v>304</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -3723,13 +4040,13 @@
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C13">
       <formula1>"Select,Bill of Supply,Normal Invoice,Overseas Tax,Overseas Non Tax"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G13">
       <formula1>$P$2:$AN$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J13">
       <formula1>$P$3:$GC$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:M8">
@@ -3743,10 +4060,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GA10"/>
+  <dimension ref="A1:GA13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4536,10 +4853,10 @@
         <v>235</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>286</v>
+        <v>233</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
@@ -4562,7 +4879,7 @@
         <v>286</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
@@ -4571,21 +4888,63 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
     </row>
-    <row r="10" spans="1:183" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:183" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>9</v>
       </c>
-      <c r="B10" s="93">
+      <c r="B10" s="59">
         <v>3</v>
       </c>
-      <c r="C10" s="100" t="s">
+      <c r="C10" s="114" t="s">
         <v>235</v>
       </c>
-      <c r="D10" s="101" t="s">
+      <c r="D10" s="115" t="s">
         <v>286</v>
       </c>
-      <c r="E10" s="99" t="s">
+      <c r="E10" s="115" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:183" x14ac:dyDescent="0.3">
+      <c r="B11" s="94">
+        <v>4</v>
+      </c>
+      <c r="C11" s="116" t="s">
+        <v>318</v>
+      </c>
+      <c r="D11" s="101" t="s">
+        <v>285</v>
+      </c>
+      <c r="E11" s="101" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:183" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="94">
+        <v>5</v>
+      </c>
+      <c r="C12" s="116" t="s">
+        <v>319</v>
+      </c>
+      <c r="D12" s="101" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" s="101" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:183" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="94">
+        <v>6</v>
+      </c>
+      <c r="C13" s="116" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" s="101" t="s">
+        <v>284</v>
+      </c>
+      <c r="E13" s="101" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -4593,13 +4952,13 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C13">
       <formula1>"STATE BANK OF INDIA(255000552232112)/22156132122/INR,BANK OF INDIA(11111112222)/23123/INR,abhyudaya co-operative bank(1234567890)/123456/INR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D13">
       <formula1>$N$4:$BS$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E13">
       <formula1>$N$3:$GA$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[IFFInvoice_Project] : Failed Screenshot Added
</commit_message>
<xml_diff>
--- a/Invoice _TestData/IFF_INVOICE_TEST_DATA.xlsx
+++ b/Invoice _TestData/IFF_INVOICE_TEST_DATA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="335">
   <si>
     <t>Basic Details</t>
   </si>
@@ -994,12 +994,6 @@
     <t>23-Jun-2023</t>
   </si>
   <si>
-    <t>06-Jul-2023</t>
-  </si>
-  <si>
-    <t>04-Jul-2023</t>
-  </si>
-  <si>
     <t>28-Jun-2023</t>
   </si>
   <si>
@@ -1021,19 +1015,22 @@
     <t>fff</t>
   </si>
   <si>
-    <t>CHN/BKG/AFI/00191/23-24</t>
-  </si>
-  <si>
     <t>01-Jul-2023</t>
   </si>
   <si>
     <t>10-Jul-2023</t>
   </si>
   <si>
-    <t>MUM/BKG/AEC/00012/2122-60</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFE/00192/23-24</t>
+    <t>14-Jul-2023</t>
+  </si>
+  <si>
+    <t>18-Jul-2023</t>
+  </si>
+  <si>
+    <t>16-Jul-2023</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFE/00195/23-24</t>
   </si>
 </sst>
 </file>
@@ -1915,6 +1912,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1926,15 +1932,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2242,7 +2239,7 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2347,11 +2344,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="114" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="112"/>
-      <c r="E2" s="113"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="116"/>
     </row>
     <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
@@ -2393,10 +2390,10 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="110"/>
+      <c r="C6" s="113"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
@@ -2485,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="91" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D8" s="64" t="s">
         <v>24</v>
@@ -2530,10 +2527,10 @@
         <v>308</v>
       </c>
       <c r="R8" s="67" t="s">
+        <v>330</v>
+      </c>
+      <c r="S8" s="67" t="s">
         <v>332</v>
-      </c>
-      <c r="S8" s="67" t="s">
-        <v>322</v>
       </c>
       <c r="T8" s="68" t="s">
         <v>313</v>
@@ -2542,7 +2539,7 @@
         <v>25</v>
       </c>
       <c r="V8" s="68" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="W8" s="80" t="s">
         <v>24</v>
@@ -2558,9 +2555,7 @@
       <c r="B9" s="46">
         <v>2</v>
       </c>
-      <c r="C9" s="92" t="s">
-        <v>334</v>
-      </c>
+      <c r="C9" s="92"/>
       <c r="D9" s="48" t="s">
         <v>24</v>
       </c>
@@ -2604,10 +2599,10 @@
         <v>309</v>
       </c>
       <c r="R9" s="52" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="S9" s="52" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="T9" s="87" t="s">
         <v>314</v>
@@ -2616,7 +2611,7 @@
         <v>25</v>
       </c>
       <c r="V9" s="51" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="W9" s="81" t="s">
         <v>24</v>
@@ -2632,9 +2627,7 @@
       <c r="B10" s="89">
         <v>3</v>
       </c>
-      <c r="C10" s="93" t="s">
-        <v>331</v>
-      </c>
+      <c r="C10" s="93"/>
       <c r="D10" s="90" t="s">
         <v>24</v>
       </c>
@@ -2678,10 +2671,10 @@
         <v>310</v>
       </c>
       <c r="R10" s="62" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="S10" s="62" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="T10" s="88" t="s">
         <v>314</v>
@@ -2690,7 +2683,7 @@
         <v>25</v>
       </c>
       <c r="V10" s="61" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="W10" s="82" t="s">
         <v>24</v>
@@ -2747,7 +2740,7 @@
         <v>310</v>
       </c>
       <c r="R11" s="107" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="S11" s="107" t="s">
         <v>311</v>
@@ -2759,7 +2752,7 @@
         <v>25</v>
       </c>
       <c r="V11" s="106" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="W11" s="109" t="s">
         <v>24</v>
@@ -2826,7 +2819,7 @@
         <v>25</v>
       </c>
       <c r="V12" s="106" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="W12" s="109" t="s">
         <v>24</v>
@@ -2893,7 +2886,7 @@
         <v>25</v>
       </c>
       <c r="V13" s="106" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="W13" s="109" t="s">
         <v>24</v>
@@ -4895,13 +4888,13 @@
       <c r="B10" s="59">
         <v>3</v>
       </c>
-      <c r="C10" s="114" t="s">
+      <c r="C10" s="110" t="s">
         <v>235</v>
       </c>
-      <c r="D10" s="115" t="s">
+      <c r="D10" s="111" t="s">
         <v>286</v>
       </c>
-      <c r="E10" s="115" t="s">
+      <c r="E10" s="111" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4909,7 +4902,7 @@
       <c r="B11" s="94">
         <v>4</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="112" t="s">
         <v>318</v>
       </c>
       <c r="D11" s="101" t="s">
@@ -4923,7 +4916,7 @@
       <c r="B12" s="94">
         <v>5</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="112" t="s">
         <v>319</v>
       </c>
       <c r="D12" s="101" t="s">
@@ -4937,7 +4930,7 @@
       <c r="B13" s="94">
         <v>6</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="112" t="s">
         <v>235</v>
       </c>
       <c r="D13" s="101" t="s">

</xml_diff>